<commit_message>
GPS module, PPS feedback 50 ohm drive, molex connectors
</commit_message>
<xml_diff>
--- a/Interface/Hardware/Assembly/assembly record.xlsx
+++ b/Interface/Hardware/Assembly/assembly record.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="207">
   <si>
     <t>designation</t>
   </si>
@@ -643,6 +643,9 @@
   </si>
   <si>
     <t>10k</t>
+  </si>
+  <si>
+    <t>47ohm</t>
   </si>
 </sst>
 </file>
@@ -2968,8 +2971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CEB6F2-06AB-416E-93B6-60BFF9DB260F}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,7 +3174,9 @@
       <c r="C12" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="16">
+        <v>43060</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
     </row>
@@ -3185,7 +3190,9 @@
       <c r="C13" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="16">
+        <v>43060</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
     </row>
@@ -3199,7 +3206,9 @@
       <c r="C14" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="16">
+        <v>46712</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
     </row>
@@ -3587,7 +3596,9 @@
       <c r="C37" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="16">
+        <v>43060</v>
+      </c>
       <c r="E37" s="10" t="s">
         <v>129</v>
       </c>
@@ -3655,7 +3666,9 @@
       <c r="C41" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="16">
+        <v>43060</v>
+      </c>
       <c r="E41" s="10" t="s">
         <v>132</v>
       </c>
@@ -3689,7 +3702,9 @@
       <c r="C43" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="16"/>
+      <c r="D43" s="16">
+        <v>43060</v>
+      </c>
       <c r="E43" s="10" t="s">
         <v>134</v>
       </c>
@@ -3741,7 +3756,9 @@
       <c r="C46" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="16"/>
+      <c r="D46" s="16">
+        <v>43060</v>
+      </c>
       <c r="E46" s="10" t="s">
         <v>190</v>
       </c>
@@ -3877,7 +3894,9 @@
         <v>196</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="D54" s="16"/>
+      <c r="D54" s="16">
+        <v>43060</v>
+      </c>
       <c r="E54" s="10" t="s">
         <v>137</v>
       </c>
@@ -4193,7 +4212,9 @@
       <c r="C72" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D72" s="16"/>
+      <c r="D72" s="16">
+        <v>43060</v>
+      </c>
       <c r="E72" s="10"/>
       <c r="F72" s="11"/>
     </row>
@@ -4463,8 +4484,12 @@
       <c r="C89" s="10">
         <v>50</v>
       </c>
-      <c r="D89" s="16"/>
-      <c r="E89" s="10"/>
+      <c r="D89" s="16">
+        <v>43060</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>206</v>
+      </c>
       <c r="F89" s="11"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -4607,7 +4632,9 @@
       <c r="C98" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D98" s="16"/>
+      <c r="D98" s="16">
+        <v>43060</v>
+      </c>
       <c r="E98" s="10" t="s">
         <v>175</v>
       </c>

</xml_diff>